<commit_message>
some corrections in the legands file2
</commit_message>
<xml_diff>
--- a/scripts/LawByState.xlsx
+++ b/scripts/LawByState.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1739f7a019139c5/touchmap/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{AD934F23-A869-4211-AF69-6DFEC9365A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6F73B23-3AFE-4DF8-B9D0-4F452C1BF4C1}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="13_ncr:1_{AD934F23-A869-4211-AF69-6DFEC9365A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EB716DA-3E90-449B-9B88-BB1CC284822D}"/>
   <bookViews>
-    <workbookView xWindow="60135" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5227" yWindow="0" windowWidth="15331" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="States" sheetId="1" r:id="rId1"/>
+    <sheet name="Bills" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">States!$A$1:$F$51</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="119">
   <si>
     <t>State</t>
   </si>
@@ -54,45 +55,27 @@
     <t>California</t>
   </si>
   <si>
-    <t>California Privacy Act &amp; California Consumer Privacy Act</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>Colorado</t>
   </si>
   <si>
-    <t>Colorado Privacy Act</t>
-  </si>
-  <si>
     <t>No PRA</t>
   </si>
   <si>
-    <t>General Exception -"The obligations imposed on controllers/processors under this act do not restrict their ability to…prevent, detect, protect against, or respond to security incidents, identity theft, fraud, harassment, or malicious, deceptive, or illegal activity; preserve the integrity of security systems; or investigate, report, or prosecute those responsible for any such action."</t>
-  </si>
-  <si>
-    <t>Connecticut Data Privacy Act</t>
-  </si>
-  <si>
     <t xml:space="preserve">General Exception </t>
   </si>
   <si>
     <t>Delaware</t>
   </si>
   <si>
-    <t>Delaware Personal Data Privacy Act</t>
-  </si>
-  <si>
     <t>General Exception</t>
   </si>
   <si>
     <t>Florida</t>
   </si>
   <si>
-    <t>Digital Bill of Rights</t>
-  </si>
-  <si>
     <t>Georgia</t>
   </si>
   <si>
@@ -105,24 +88,15 @@
     <t>Bill Stage</t>
   </si>
   <si>
-    <t>BIPA</t>
-  </si>
-  <si>
     <t>High Litigation Risk - Collection requires notice and signed waiver - Facebook had a recent breakthrough by arguing momentary capture does not violate the law &amp; the judgement is in pending appeal.</t>
   </si>
   <si>
     <t>Indiana</t>
   </si>
   <si>
-    <t>Indiana Consumer Data Protection Act</t>
-  </si>
-  <si>
     <t>Iowa</t>
   </si>
   <si>
-    <t>Iowa Consumer Data Protection Act</t>
-  </si>
-  <si>
     <t>Kansas</t>
   </si>
   <si>
@@ -138,21 +112,12 @@
     <t>Massachusetts</t>
   </si>
   <si>
-    <t>BILL S 25</t>
-  </si>
-  <si>
     <t>Michigan</t>
   </si>
   <si>
-    <t>No Exception - Strict Data Security Requirements -likely carruy on to final law due to similar provision in related law -Massachusetts Data Security Law (201 CMR 17.00)</t>
-  </si>
-  <si>
     <t>Minnesota</t>
   </si>
   <si>
-    <t>Minnesota Consumer Data Privacy Act</t>
-  </si>
-  <si>
     <t xml:space="preserve">No Exception </t>
   </si>
   <si>
@@ -171,16 +136,10 @@
     <t>Montana</t>
   </si>
   <si>
-    <t xml:space="preserve">Montana Consumer Data Privacy Act </t>
-  </si>
-  <si>
     <t>Nebraska</t>
   </si>
   <si>
     <t>Nebraska Data Privacy Act</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limited class action risk  &amp; sharing biometrics considered sales and therefore additional obligations </t>
   </si>
   <si>
     <r>
@@ -236,9 +195,6 @@
     <t>New Hampshire</t>
   </si>
   <si>
-    <t>Expectation of Privacy</t>
-  </si>
-  <si>
     <t>New Jersey</t>
   </si>
   <si>
@@ -266,12 +222,6 @@
     <t>Oregon</t>
   </si>
   <si>
-    <t xml:space="preserve">Oregon Consumer Privacy Act </t>
-  </si>
-  <si>
-    <t>YEs</t>
-  </si>
-  <si>
     <t>Pennsylvania</t>
   </si>
   <si>
@@ -284,15 +234,9 @@
     <t>South Carolina</t>
   </si>
   <si>
-    <t xml:space="preserve">Tennessee Information Protection Act </t>
-  </si>
-  <si>
     <t>Texas</t>
   </si>
   <si>
-    <t>Texas Data Privacy and Security Act</t>
-  </si>
-  <si>
     <t xml:space="preserve">Portland City law (Portland City Code 34.10) prohibit Biometrics in City Limits, General exception for State Law. </t>
   </si>
   <si>
@@ -314,9 +258,6 @@
     <t>Washington</t>
   </si>
   <si>
-    <t>WA Biometrics</t>
-  </si>
-  <si>
     <t>Special Exception -"The law provides an exemption for enrolling a biometric identifier and storing it in a biometric system in furtherance of a security purpose, which is further defined as ‘preventing shoplifting, fraud, or any other misappropriation or theft of a thing of value, including tangible and intangible goods, services, and other purposes in furtherance of protecting the security or integrity of software, accounts, applications, online services, or any person.’"</t>
   </si>
   <si>
@@ -332,9 +273,6 @@
     <t>Data Security &amp; DPIA</t>
   </si>
   <si>
-    <t>Data Security - Processor should establish, implement, and maintain reasonable administrative, technical, and physical data security practices appropriate to the volume and nature of the personal data at issue &amp; DPIA</t>
-  </si>
-  <si>
     <t>Security &amp; DPIA</t>
   </si>
   <si>
@@ -387,6 +325,111 @@
   </si>
   <si>
     <t>Vermont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limited class action risk  &amp; sharing biometrics considered sale and therefore additional obligations </t>
+  </si>
+  <si>
+    <t>Data Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This law may not strictly apply to retail theft prevention use cases as the law regulates online activity but the law indicates a pattern similar to Colorado type approach towards biometric regulations. </t>
+  </si>
+  <si>
+    <t>No Exception - Strict Data Security Requirements -likely carry on to final law due to similar provision in related law -Massachusetts Data Security Law (201 CMR 17.00)</t>
+  </si>
+  <si>
+    <t>BillID</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LastUpdated </t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>SB 473</t>
+  </si>
+  <si>
+    <t>Title details</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>Key Points</t>
+  </si>
+  <si>
+    <t>SB 1234</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PDF: Texas Data Privacy and Security Act|https://touchmap.s3.us-east-2.amazonaws.com/Texas+Data+Privacy+and+Security+Act.pdf] </t>
+  </si>
+  <si>
+    <t>[PDF: BIPA|https://touchmap.s3.us-east-2.amazonaws.com/BIPA.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:California Privacy Act &amp; California Consumer Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/California+-+California+Consumer+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Colorado Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Colorado+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Connecticut Data Privacy Act |https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Connecticut+Personal+Data+Privacy+and+Online+Monitoring+Act.pdf]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PDF: Delaware Personal Data Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Delaware+Personal+Data+Privacy+Act+(DPDPA).pdf] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PDF: Digital Bill of Rights|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Florida+Bill+of+Rights+aka+Privacy+Act.pdf] </t>
+  </si>
+  <si>
+    <t>[PDF: Indiana Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Indiana+Privay+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Iowa Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Iowa+Privacy+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Mass Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Mass+Privacy+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Minnesota Data Privacy|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Minnesota+Data+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Montana Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Montana+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: New Hampshire Expectation of Privacy|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/New+Hamshare+Expectation+of+Privacy.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: New Jersey Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/New+Jersey+Privacy+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Oregon Consumer Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Oregon+Consumer+Privacy+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Tennessee Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Tenesee+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PDF: WA Privacy Law - Biometrics Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/WA+Privacy+Law+-Aka+Biometrics+law.pdf] </t>
   </si>
 </sst>
 </file>
@@ -513,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -562,6 +605,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,16 +894,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.86328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.46484375" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.265625" style="2" customWidth="1"/>
     <col min="5" max="5" width="49.6640625" style="2" customWidth="1"/>
@@ -872,19 +920,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -904,7 +952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -924,9 +972,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -944,7 +992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -964,149 +1012,149 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
+      <c r="B7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
+      <c r="B11" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>4</v>
@@ -1126,67 +1174,67 @@
     </row>
     <row r="14" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>4</v>
@@ -1206,439 +1254,439 @@
     </row>
     <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A24" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="5" t="s">
+      <c r="F26" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="13" t="s">
-        <v>46</v>
-      </c>
       <c r="B27" s="3" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A30" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A31" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A38" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B38" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="B39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>4</v>
@@ -1646,27 +1694,27 @@
     </row>
     <row r="40" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="13" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>4</v>
@@ -1684,9 +1732,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>4</v>
@@ -1704,69 +1752,69 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A43" s="10" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="10" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>4</v>
@@ -1778,7 +1826,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>4</v>
@@ -1786,19 +1834,19 @@
     </row>
     <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A47" s="13" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>4</v>
@@ -1806,28 +1854,28 @@
     </row>
     <row r="48" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A48" s="10" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="B49" s="2" t="s">
         <v>4</v>
       </c>
@@ -1838,15 +1886,15 @@
         <v>4</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>4</v>
@@ -1858,15 +1906,15 @@
         <v>4</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" s="8" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>4</v>
@@ -1909,25 +1957,138 @@
       <c r="B59" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F51" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="[PDF: BIPA|https://touchmap.s3.us-east-2.amazonaws.com/BIPA.pdf]"/>
+        <filter val="[PDF: Colorado Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Colorado+Privacy+Act.pdf]"/>
+        <filter val="[PDF: Connecticut Data Privacy Act |https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Connecticut+Personal+Data+Privacy+and+Online+Monitoring+Act.pdf]"/>
+        <filter val="[PDF: Delaware Personal Data Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Delaware+Personal+Data+Privacy+Act+(DPDPA).pdf]"/>
+        <filter val="[PDF: Digital Bill of Rights|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Florida+Bill+of+Rights+aka+Privacy+Act.pdf]"/>
+        <filter val="[PDF: Indiana Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Indiana+Privay+Law.pdf]"/>
+        <filter val="[PDF: Iowa Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Iowa+Privacy+Law.pdf]"/>
+        <filter val="[PDF: Mass Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Mass+Privacy+Law.pdf]"/>
+        <filter val="[PDF: Texas Data Privacy and Security Act|https://touchmap.s3.us-east-2.amazonaws.com/Texas+Data+Privacy+and+Security+Act.pdf]"/>
+        <filter val="[PDF:California Privacy Act &amp; California Consumer Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/California+-+California+Consumer+Privacy+Act.pdf]"/>
+        <filter val="Kentucky Consumer Data Protection Act"/>
+        <filter val="Nebraska Data Privacy Act"/>
+        <filter val="Rhode Island Data Transparency and Privacy Protection Act"/>
+        <filter val="Utah Consumer Privacy Act"/>
+        <filter val="Virginia Consumer Data Protection Act"/>
+        <filter val="WA Biometrics"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" xr:uid="{4E9F0E54-0F08-405F-8B74-00273CFF7750}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{8DA464AA-7553-4894-973F-8F9124A6BBD1}"/>
+    <hyperlink ref="B15" r:id="rId1" display="Indiana Consumer Data Protection Act" xr:uid="{4E9F0E54-0F08-405F-8B74-00273CFF7750}"/>
+    <hyperlink ref="B16" r:id="rId2" display="Iowa Consumer Data Protection Act" xr:uid="{8DA464AA-7553-4894-973F-8F9124A6BBD1}"/>
     <hyperlink ref="B18" r:id="rId3" xr:uid="{9D531AD9-A581-45C6-A557-C416674C7063}"/>
-    <hyperlink ref="B22" r:id="rId4" xr:uid="{3D086796-7CD2-4B01-94A4-B1F866F35738}"/>
-    <hyperlink ref="B24" r:id="rId5" xr:uid="{A81962F2-A590-4E92-8CD1-3A30F3096351}"/>
-    <hyperlink ref="B27" r:id="rId6" xr:uid="{A6798D2B-D7B6-40F4-BFD2-601EFD4DDA99}"/>
-    <hyperlink ref="B28" r:id="rId7" xr:uid="{D1BDCD38-1646-4FCC-BB69-FD036C1FA921}"/>
-    <hyperlink ref="B30" r:id="rId8" xr:uid="{7493D007-812B-426D-AD80-9C8D298ECE97}"/>
-    <hyperlink ref="B31" r:id="rId9" xr:uid="{9197E8EB-4DA8-442D-B9E3-FE4534914BE5}"/>
-    <hyperlink ref="B38" r:id="rId10" xr:uid="{6AF69A3E-7CAF-4F62-AAB8-4C96E3A2382B}"/>
-    <hyperlink ref="B40" r:id="rId11" xr:uid="{2A71332F-9BE0-4373-939F-3518AD87D665}"/>
-    <hyperlink ref="B43" r:id="rId12" xr:uid="{16F0FF51-361D-49AF-A8CD-1AD33FF24D57}"/>
-    <hyperlink ref="B44" r:id="rId13" xr:uid="{8A36D1A6-FBC2-4B00-A9C5-B8DC8E928D9E}"/>
-    <hyperlink ref="B45" r:id="rId14" xr:uid="{DB0CF2B6-1FA6-4442-9131-257A9DDEFE77}"/>
-    <hyperlink ref="B47" r:id="rId15" xr:uid="{148D8731-FCD1-426D-9FC4-393703E1AF4D}"/>
+    <hyperlink ref="B24" r:id="rId4" display="Minnesota Consumer Data Privacy Act" xr:uid="{A81962F2-A590-4E92-8CD1-3A30F3096351}"/>
+    <hyperlink ref="B28" r:id="rId5" xr:uid="{D1BDCD38-1646-4FCC-BB69-FD036C1FA921}"/>
+    <hyperlink ref="B40" r:id="rId6" xr:uid="{2A71332F-9BE0-4373-939F-3518AD87D665}"/>
+    <hyperlink ref="B44" r:id="rId7" display="Texas Data Privacy and Security Act" xr:uid="{8A36D1A6-FBC2-4B00-A9C5-B8DC8E928D9E}"/>
+    <hyperlink ref="B45" r:id="rId8" xr:uid="{DB0CF2B6-1FA6-4442-9131-257A9DDEFE77}"/>
+    <hyperlink ref="B47" r:id="rId9" xr:uid="{148D8731-FCD1-426D-9FC4-393703E1AF4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06456C32-F4AC-4325-8B3B-697BE0C61C36}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="12.53125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" customWidth="1"/>
+    <col min="5" max="5" width="12.9296875" customWidth="1"/>
+    <col min="6" max="6" width="13.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="17">
+        <v>45337</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="17">
+        <v>45337</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some corrections in the legands file7
</commit_message>
<xml_diff>
--- a/scripts/LawByState.xlsx
+++ b/scripts/LawByState.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1739f7a019139c5/touchmap/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="13_ncr:1_{AD934F23-A869-4211-AF69-6DFEC9365A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EB716DA-3E90-449B-9B88-BB1CC284822D}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="13_ncr:1_{AD934F23-A869-4211-AF69-6DFEC9365A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{425B1CE1-0DEE-4928-B334-02D399B8171A}"/>
   <bookViews>
-    <workbookView xWindow="5227" yWindow="0" windowWidth="15331" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="56415" yWindow="870" windowWidth="15330" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="States" sheetId="1" r:id="rId1"/>
@@ -381,55 +381,55 @@
     <t>TX</t>
   </si>
   <si>
-    <t xml:space="preserve">[PDF: Texas Data Privacy and Security Act|https://touchmap.s3.us-east-2.amazonaws.com/Texas+Data+Privacy+and+Security+Act.pdf] </t>
-  </si>
-  <si>
-    <t>[PDF: BIPA|https://touchmap.s3.us-east-2.amazonaws.com/BIPA.pdf]</t>
-  </si>
-  <si>
     <t>[PDF:California Privacy Act &amp; California Consumer Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/California+-+California+Consumer+Privacy+Act.pdf]</t>
   </si>
   <si>
-    <t>[PDF: Colorado Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Colorado+Privacy+Act.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: Connecticut Data Privacy Act |https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Connecticut+Personal+Data+Privacy+and+Online+Monitoring+Act.pdf]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[PDF: Delaware Personal Data Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Delaware+Personal+Data+Privacy+Act+(DPDPA).pdf] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[PDF: Digital Bill of Rights|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Florida+Bill+of+Rights+aka+Privacy+Act.pdf] </t>
-  </si>
-  <si>
-    <t>[PDF: Indiana Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Indiana+Privay+Law.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: Iowa Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Iowa+Privacy+Law.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: Mass Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Mass+Privacy+Law.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: Minnesota Data Privacy|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Minnesota+Data+Privacy+Act.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: Montana Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Montana+Privacy+Act.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: New Hampshire Expectation of Privacy|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/New+Hamshare+Expectation+of+Privacy.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: New Jersey Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/New+Jersey+Privacy+Law.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: Oregon Consumer Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Oregon+Consumer+Privacy+Law.pdf]</t>
-  </si>
-  <si>
-    <t>[PDF: Tennessee Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Tenesee+Privacy+Act.pdf]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[PDF: WA Privacy Law - Biometrics Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/WA+Privacy+Law+-Aka+Biometrics+law.pdf] </t>
+    <t>[PDF:Indiana Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Indiana+Privay+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Colorado Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Colorado+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Connecticut Data Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Connecticut+Personal+Data+Privacy+and+Online+Monitoring+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Delaware Personal Data Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Delaware+Personal+Data+Privacy+Act+(DPDPA).pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Digital Bill of Rights|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Florida+Bill+of+Rights+aka+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:BIPA|https://touchmap.s3.us-east-2.amazonaws.com/BIPA.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Iowa Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Iowa+Privacy+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Mass Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Mass+Privacy+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Minnesota Data Privacy|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Minnesota+Data+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Montana Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Montana+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:New Hampshire Expectation of Privacy|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/New+Hamshare+Expectation+of+Privacy.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:New Jersey Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/New+Jersey+Privacy+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Oregon Consumer Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Oregon+Consumer+Privacy+Law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Tennessee Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Tenesee+Privacy+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:Texas Data Privacy and Security Act|https://touchmap.s3.us-east-2.amazonaws.com/Texas+Data+Privacy+and+Security+Act.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF:WA Privacy Law - Biometrics Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/WA+Privacy+Law+-Aka+Biometrics+law.pdf]</t>
   </si>
 </sst>
 </file>
@@ -894,11 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -932,7 +931,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -952,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -972,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>73</v>
       </c>
@@ -992,7 +991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>72</v>
@@ -1032,12 +1031,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -1057,7 +1056,7 @@
         <v>82</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -1077,7 +1076,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -1097,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>8</v>
@@ -1112,7 +1111,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1132,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1152,7 +1151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1177,7 +1176,7 @@
         <v>74</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>72</v>
@@ -1197,7 +1196,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
@@ -1217,7 +1216,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
@@ -1232,7 +1231,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
@@ -1292,7 +1291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
@@ -1332,12 +1331,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>72</v>
@@ -1352,7 +1351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>72</v>
@@ -1392,7 +1391,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1412,7 +1411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>33</v>
       </c>
@@ -1437,7 +1436,7 @@
         <v>34</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
@@ -1472,7 +1471,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1497,7 +1496,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>8</v>
@@ -1517,7 +1516,7 @@
         <v>40</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>8</v>
@@ -1532,7 +1531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
@@ -1572,7 +1571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
         <v>44</v>
       </c>
@@ -1592,7 +1591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>76</v>
       </c>
@@ -1612,7 +1611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>79</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>48</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>8</v>
@@ -1672,7 +1671,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
         <v>49</v>
       </c>
@@ -1712,7 +1711,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>52</v>
       </c>
@@ -1732,7 +1731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>77</v>
       </c>
@@ -1757,7 +1756,7 @@
         <v>75</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>8</v>
@@ -1777,7 +1776,7 @@
         <v>53</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>8</v>
@@ -1812,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>83</v>
       </c>
@@ -1872,7 +1871,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>80</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
         <v>63</v>
       </c>
@@ -1912,7 +1911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="8" t="s">
         <v>64</v>
       </c>
@@ -1957,28 +1956,7 @@
       <c r="B59" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F51" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="[PDF: BIPA|https://touchmap.s3.us-east-2.amazonaws.com/BIPA.pdf]"/>
-        <filter val="[PDF: Colorado Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Colorado+Privacy+Act.pdf]"/>
-        <filter val="[PDF: Connecticut Data Privacy Act |https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Connecticut+Personal+Data+Privacy+and+Online+Monitoring+Act.pdf]"/>
-        <filter val="[PDF: Delaware Personal Data Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Delaware+Personal+Data+Privacy+Act+(DPDPA).pdf]"/>
-        <filter val="[PDF: Digital Bill of Rights|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Florida+Bill+of+Rights+aka+Privacy+Act.pdf]"/>
-        <filter val="[PDF: Indiana Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Indiana+Privay+Law.pdf]"/>
-        <filter val="[PDF: Iowa Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Iowa+Privacy+Law.pdf]"/>
-        <filter val="[PDF: Mass Privacy Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Mass+Privacy+Law.pdf]"/>
-        <filter val="[PDF: Texas Data Privacy and Security Act|https://touchmap.s3.us-east-2.amazonaws.com/Texas+Data+Privacy+and+Security+Act.pdf]"/>
-        <filter val="[PDF:California Privacy Act &amp; California Consumer Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/California+-+California+Consumer+Privacy+Act.pdf]"/>
-        <filter val="Kentucky Consumer Data Protection Act"/>
-        <filter val="Nebraska Data Privacy Act"/>
-        <filter val="Rhode Island Data Transparency and Privacy Protection Act"/>
-        <filter val="Utah Consumer Privacy Act"/>
-        <filter val="Virginia Consumer Data Protection Act"/>
-        <filter val="WA Biometrics"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1" display="Indiana Consumer Data Protection Act" xr:uid="{4E9F0E54-0F08-405F-8B74-00273CFF7750}"/>
     <hyperlink ref="B16" r:id="rId2" display="Iowa Consumer Data Protection Act" xr:uid="{8DA464AA-7553-4894-973F-8F9124A6BBD1}"/>

</xml_diff>

<commit_message>
type correction in TX file
</commit_message>
<xml_diff>
--- a/scripts/LawByState.xlsx
+++ b/scripts/LawByState.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1739f7a019139c5/touchmap/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="13_ncr:1_{AD934F23-A869-4211-AF69-6DFEC9365A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCBE172D-F862-464A-9B79-2613DB4A4B9D}"/>
+  <xr:revisionPtr revIDLastSave="237" documentId="13_ncr:1_{AD934F23-A869-4211-AF69-6DFEC9365A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3F26CC2-C78C-48BF-B075-E54952EE0637}"/>
   <bookViews>
-    <workbookView xWindow="56415" yWindow="870" windowWidth="15330" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="States" sheetId="1" r:id="rId1"/>
@@ -396,9 +396,6 @@
     <t>[PDF: Digital Bill of Rights|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Florida+Bill+of+Rights+aka+Privacy+Act.pdf]</t>
   </si>
   <si>
-    <t>[PDF: BIPA|https://touchmap.s3.us-east-2.amazonaws.com/BIPA.pdf]</t>
-  </si>
-  <si>
     <t>[PDF: Indiana Consumer Data Protection Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Indiana+Privay+Law.pdf]</t>
   </si>
   <si>
@@ -426,10 +423,13 @@
     <t>[PDF: Tennessee Privacy Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Tenesee+Privacy+Act.pdf]</t>
   </si>
   <si>
-    <t>[PDF: Texas Data Privacy and Security Act|https://touchmap.s3.us-east-2.amazonaws.com/Texas+Data+Privacy+and+Security+Act.pdf]</t>
-  </si>
-  <si>
     <t>[PDF: WA Privacy Law - Biometrics Law|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/WA+Privacy+Law+-Aka+Biometrics+law.pdf]</t>
+  </si>
+  <si>
+    <t>[PDF: Texas Data Privacy and Security Act|https://touchmap.s3.us-east-2.amazonaws.com/state_laws/Texas+Data+Privacy+and+Security+Act.pdf]</t>
+  </si>
+  <si>
+    <t>BIPA</t>
   </si>
 </sst>
 </file>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1176,7 +1176,7 @@
         <v>74</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>72</v>
@@ -1196,7 +1196,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
@@ -1216,7 +1216,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
@@ -1336,7 +1336,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>72</v>
@@ -1376,7 +1376,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>72</v>
@@ -1436,7 +1436,7 @@
         <v>34</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
@@ -1496,7 +1496,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>8</v>
@@ -1516,7 +1516,7 @@
         <v>40</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>8</v>
@@ -1656,7 +1656,7 @@
         <v>48</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>8</v>
@@ -1756,7 +1756,7 @@
         <v>75</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>8</v>
@@ -1856,7 +1856,7 @@
         <v>60</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
adding dark green to Washington
</commit_message>
<xml_diff>
--- a/scripts/LawByState.xlsx
+++ b/scripts/LawByState.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1739f7a019139c5/touchmap/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalan\OneDrive\touchmap\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="13_ncr:1_{AD934F23-A869-4211-AF69-6DFEC9365A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2527CBF-2AD0-4A43-8718-A361669D28D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A65599C-AC1B-4F08-9F10-E71CA4E305E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="States" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +543,12 @@
         <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -556,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -610,6 +616,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,10 +634,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -896,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1852,7 +1857,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="19" t="s">
         <v>60</v>
       </c>
       <c r="B48" s="7" t="s">

</xml_diff>